<commit_message>
Ny alternativ i soknad
</commit_message>
<xml_diff>
--- a/kgdata.xlsx
+++ b/kgdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="foresatt" sheetId="1" state="visible" r:id="rId3"/>
@@ -405,14 +405,18 @@
   </sheetPr>
   <dimension ref="B1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,11 +454,19 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -612,6 +624,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.48"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -640,10 +656,23 @@
   <dimension ref="B1:M1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.49"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">

</xml_diff>